<commit_message>
caricamento dati multiple poles and right half time zero
</commit_message>
<xml_diff>
--- a/Benchmark_System/Multiple_Equals_poles8/Multiple Equal Poles8.xlsx
+++ b/Benchmark_System/Multiple_Equals_poles8/Multiple Equal Poles8.xlsx
@@ -152,16 +152,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>6.2205449466230629</v>
+        <v>6.2205449478915495</v>
       </c>
       <c r="C2">
-        <v>10.088932515629818</v>
+        <v>10.088932515975207</v>
       </c>
       <c r="D2">
-        <v>7.7910835671262566</v>
+        <v>7.7910835671158161</v>
       </c>
       <c r="E2">
-        <v>4.2627870527887604</v>
+        <v>4.2627860862114568</v>
       </c>
     </row>
     <row r="3">
@@ -169,16 +169,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.90468096333319714</v>
+        <v>0.90468654188861353</v>
       </c>
       <c r="C3">
-        <v>1.300270571156273</v>
+        <v>1.3002718982054766</v>
       </c>
       <c r="D3">
-        <v>0.91863534888086251</v>
+        <v>0.91863158209723739</v>
       </c>
       <c r="E3">
-        <v>1.8254958942809334</v>
+        <v>1.8260152612626817</v>
       </c>
     </row>
     <row r="4">
@@ -186,16 +186,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4.6341727549318001</v>
+        <v>4.6341749033787023</v>
       </c>
       <c r="C4">
-        <v>5.0657754558878141</v>
+        <v>5.0657786490690713</v>
       </c>
       <c r="D4">
-        <v>6.4329881806166229</v>
+        <v>6.4329677061929003</v>
       </c>
       <c r="E4">
-        <v>6.978147906187008</v>
+        <v>6.9795806742906992</v>
       </c>
     </row>
     <row r="5">
@@ -203,16 +203,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2.5079822461424737</v>
+        <v>2.5079867320948721</v>
       </c>
       <c r="C5">
-        <v>2.239027682470816</v>
+        <v>2.2390278274351099</v>
       </c>
       <c r="D5">
-        <v>2.3199508602626815</v>
+        <v>2.3199095589483352</v>
       </c>
       <c r="E5">
-        <v>2.0353189678828132</v>
+        <v>2.0348548335227075</v>
       </c>
     </row>
     <row r="6">
@@ -220,7 +220,7 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>3.100233442200242</v>
+        <v>3.1003992135261251</v>
       </c>
     </row>
     <row r="7">
@@ -262,16 +262,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>25079.822461424734</v>
+        <v>25079.867320948721</v>
       </c>
       <c r="C9">
-        <v>22390.276824708159</v>
+        <v>22390.278274351098</v>
       </c>
       <c r="D9">
-        <v>23199.508602626815</v>
+        <v>23199.09558948335</v>
       </c>
       <c r="E9">
-        <v>20353.18967882813</v>
+        <v>20348.548335227075</v>
       </c>
     </row>
     <row r="10">
@@ -279,7 +279,7 @@
         <v>9</v>
       </c>
       <c r="E10">
-        <v>31002.334422002419</v>
+        <v>31003.992135261251</v>
       </c>
     </row>
     <row r="11">
@@ -287,16 +287,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>4.3343009059007755</v>
+        <v>4.3342674124273604</v>
       </c>
       <c r="C11">
-        <v>6.1022577064865002</v>
+        <v>6.1022571540750352</v>
       </c>
       <c r="D11">
-        <v>5.1161722900258777</v>
+        <v>5.1161769500034797</v>
       </c>
       <c r="E11">
-        <v>3.022070630224412</v>
+        <v>3.0215229534704662</v>
       </c>
     </row>
     <row r="12">
@@ -304,16 +304,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>25.85061260490323</v>
+        <v>25.850573792598141</v>
       </c>
       <c r="C12">
-        <v>29.976289193078525</v>
+        <v>29.97628653383693</v>
       </c>
       <c r="D12">
-        <v>27.243196360038493</v>
+        <v>27.243215089760614</v>
       </c>
       <c r="E12">
-        <v>21.747079621821783</v>
+        <v>21.74758906882867</v>
       </c>
     </row>
     <row r="13">
@@ -321,16 +321,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>6.4452562569303762</v>
+        <v>6.4456210257433533</v>
       </c>
       <c r="C13">
-        <v>6.6863396837880451</v>
+        <v>6.6863112203408237</v>
       </c>
       <c r="D13">
-        <v>6.1530662561920302</v>
+        <v>6.1533091811755591</v>
       </c>
       <c r="E13">
-        <v>7.3715620643193702</v>
+        <v>7.3800098108694145</v>
       </c>
     </row>
     <row r="14">
@@ -355,16 +355,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1.0644525625693038</v>
+        <v>1.0644562102574333</v>
       </c>
       <c r="C15">
-        <v>1.0668633968378805</v>
+        <v>1.0668631122034082</v>
       </c>
       <c r="D15">
-        <v>1.0615306625619081</v>
+        <v>1.0615330918117374</v>
       </c>
       <c r="E15">
-        <v>1.0737156206431937</v>
+        <v>1.0738000981086941</v>
       </c>
     </row>
     <row r="16">
@@ -372,16 +372,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>10.376559663410335</v>
+        <v>10.376554596361856</v>
       </c>
       <c r="C16">
-        <v>15.538492320125714</v>
+        <v>15.538486585096859</v>
       </c>
       <c r="D16">
-        <v>12.582039103366681</v>
+        <v>12.582062933265011</v>
       </c>
       <c r="E16">
-        <v>7.1433899446035243</v>
+        <v>7.1419521408909485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>